<commit_message>
Updated timing for manual mode
</commit_message>
<xml_diff>
--- a/VirutalOperatingSystem/Graph Data.csv.xlsx
+++ b/VirutalOperatingSystem/Graph Data.csv.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9084"/>
   </bookViews>
   <sheets>
-    <sheet name="Average Waiting Time" sheetId="2" r:id="rId1"/>
+    <sheet name="Chart1" sheetId="2" r:id="rId1"/>
     <sheet name="Graph Data" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
@@ -764,7 +764,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -778,7 +778,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Average Waiting Time</a:t>
+              <a:t>Total Time</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -796,7 +796,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -822,7 +822,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:ln w="28575" cap="rnd">
+            <a:ln w="22225" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
@@ -831,7 +831,20 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="none"/>
+            <c:symbol val="diamond"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
           </c:marker>
           <c:cat>
             <c:strRef>
@@ -1005,171 +1018,171 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Graph Data'!$C$2:$C$55</c:f>
+              <c:f>'Graph Data'!$B$2:$B$55</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="54"/>
                 <c:pt idx="0">
-                  <c:v>34</c:v>
+                  <c:v>30464</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>67</c:v>
+                  <c:v>32288</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>33</c:v>
+                  <c:v>30350</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>29409</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>29175</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>29272</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>29214</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>29259</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1</c:v>
+                  <c:v>29356</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1948</c:v>
+                  <c:v>30241</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1968</c:v>
+                  <c:v>30565</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1953</c:v>
+                  <c:v>30357</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>69</c:v>
+                  <c:v>15304</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>67</c:v>
+                  <c:v>15282</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>67</c:v>
+                  <c:v>15143</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1</c:v>
+                  <c:v>15138</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1</c:v>
+                  <c:v>15210</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1</c:v>
+                  <c:v>15214</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1966</c:v>
+                  <c:v>30524</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1946</c:v>
+                  <c:v>30224</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>1977</c:v>
+                  <c:v>30709</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>67</c:v>
+                  <c:v>15196</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>68</c:v>
+                  <c:v>15137</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>68</c:v>
+                  <c:v>15147</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1</c:v>
+                  <c:v>15072</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1</c:v>
+                  <c:v>15122</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1</c:v>
+                  <c:v>15164</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>5413</c:v>
+                  <c:v>30446</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>5447</c:v>
+                  <c:v>30600</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>5383</c:v>
+                  <c:v>30279</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>1881</c:v>
+                  <c:v>15138</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>1877</c:v>
+                  <c:v>15127</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>1882</c:v>
+                  <c:v>15135</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>135</c:v>
+                  <c:v>8184</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>145</c:v>
+                  <c:v>8147</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>135</c:v>
+                  <c:v>8128</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>5364</c:v>
+                  <c:v>30251</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>5407</c:v>
+                  <c:v>30465</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>5383</c:v>
+                  <c:v>30296</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>1891</c:v>
+                  <c:v>15195</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>1876</c:v>
+                  <c:v>15130</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>1873</c:v>
+                  <c:v>15071</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>134</c:v>
+                  <c:v>8060</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>134</c:v>
+                  <c:v>8063</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>134</c:v>
+                  <c:v>8071</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>10709</c:v>
+                  <c:v>30536</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>10704</c:v>
+                  <c:v>30530</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>10638</c:v>
+                  <c:v>30299</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>4763</c:v>
+                  <c:v>15343</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>4759</c:v>
+                  <c:v>15335</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>4677</c:v>
+                  <c:v>15071</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>1770</c:v>
+                  <c:v>8190</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>1778</c:v>
+                  <c:v>8208</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>1760</c:v>
+                  <c:v>8136</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1177,7 +1190,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-E520-4BCF-8387-01BB955BFA60}"/>
+              <c16:uniqueId val="{00000000-0585-4F20-AE67-E971CEAEBF13}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1191,29 +1204,43 @@
         </c:dLbls>
         <c:hiLowLines>
           <c:spPr>
+            <a:ln w="9525">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="50000"/>
+                  <a:lumOff val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="385078016"/>
+        <c:axId val="385079000"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="385078016"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
                 <a:schemeClr val="tx1">
-                  <a:lumMod val="75000"/>
-                  <a:lumOff val="25000"/>
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-        </c:hiLowLines>
-        <c:smooth val="0"/>
-        <c:axId val="446331672"/>
-        <c:axId val="446332328"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="446331672"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
+        </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -1221,7 +1248,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -1235,7 +1262,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Number of Pages - Page Size - Number of CPUS - Sorting Method</a:t>
+                  <a:t>Number of Pages - Page Size - Number of CPUs - Sorting Method Used</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1253,7 +1280,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -1291,7 +1318,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -1306,7 +1333,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="446332328"/>
+        <c:crossAx val="385079000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1314,26 +1341,12 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="446332328"/>
+        <c:axId val="385079000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
         <c:title>
           <c:tx>
             <c:rich>
@@ -1341,7 +1354,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -1355,7 +1368,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Time Spent on Queue</a:t>
+                  <a:t>Elapsed Time (Microseconds)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1373,7 +1386,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -1390,13 +1403,19 @@
           </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln>
-            <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -1420,7 +1439,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="446331672"/>
+        <c:crossAx val="385078016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1433,7 +1452,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="r"/>
+      <c:legendPos val="t"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1469,7 +1488,7 @@
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:schemeClr val="bg1"/>
+      <a:schemeClr val="lt1"/>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
@@ -1492,6 +1511,7 @@
       <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
+  <c:userShapes r:id="rId3"/>
 </c:chartSpace>
 </file>
 
@@ -1536,7 +1556,7 @@
 </file>
 
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="239">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -1547,7 +1567,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
@@ -1570,18 +1590,18 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="800" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
   </cs:categoryAxis>
   <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="bg1"/>
+        <a:schemeClr val="lt1"/>
       </a:solidFill>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
@@ -1593,7 +1613,7 @@
         <a:round/>
       </a:ln>
     </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" kern="1200"/>
   </cs:chartArea>
   <cs:dataLabel>
     <cs:lnRef idx="0"/>
@@ -1601,11 +1621,11 @@
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
   </cs:dataLabel>
   <cs:dataLabelCallout>
     <cs:lnRef idx="0"/>
@@ -1637,12 +1657,12 @@
   </cs:dataLabelCallout>
   <cs:dataPoint>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -1652,12 +1672,12 @@
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -1669,13 +1689,13 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
+    <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+      <a:ln w="22225" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -1687,12 +1707,12 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1">
+    <cs:fillRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:fillRef>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -1702,18 +1722,19 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointMarkerLayout size="6"/>
   <cs:dataPointWireframe>
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
+    <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -1735,15 +1756,13 @@
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="15000"/>
             <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1758,15 +1777,15 @@
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -1777,17 +1796,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:dropLine>
@@ -1796,10 +1814,10 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
@@ -1815,21 +1833,15 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
   </cs:floor>
   <cs:gridlineMajor>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -1848,17 +1860,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln>
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="5000"/>
             <a:lumOff val="95000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:gridlineMinor>
@@ -1867,17 +1878,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:hiLoLine>
@@ -1886,17 +1896,16 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
             <a:lumOff val="65000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:leaderLine>
@@ -1917,7 +1926,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:plotArea>
   <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
@@ -1925,7 +1934,7 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:plotArea3D>
   <cs:seriesAxis>
@@ -1938,6 +1947,17 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:seriesAxis>
   <cs:seriesLine>
@@ -1945,10 +1965,10 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="35000"/>
@@ -1969,7 +1989,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -1978,14 +1998,14 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:prstDash val="sysDot"/>
+        <a:prstDash val="sysDash"/>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -1999,7 +2019,7 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
+    <cs:defRPr sz="800" kern="1200"/>
   </cs:trendlineLabel>
   <cs:upBar>
     <cs:lnRef idx="0"/>
@@ -2015,8 +2035,8 @@
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
       </a:ln>
@@ -2032,6 +2052,17 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -2039,14 +2070,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -2055,7 +2080,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="87" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="81" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2087,6 +2112,96 @@
     <xdr:clientData/>
   </xdr:absoluteAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.76456</cdr:x>
+      <cdr:y>0.69508</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>0.78736</cdr:x>
+      <cdr:y>0.79994</cdr:y>
+    </cdr:to>
+    <cdr:cxnSp macro="">
+      <cdr:nvCxnSpPr>
+        <cdr:cNvPr id="5" name="Straight Arrow Connector 4"/>
+        <cdr:cNvCxnSpPr/>
+      </cdr:nvCxnSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" flipV="1">
+          <a:off x="6622815" y="4365037"/>
+          <a:ext cx="197555" cy="658519"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </cdr:spPr>
+      <cdr:style>
+        <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </cdr:style>
+    </cdr:cxnSp>
+  </cdr:relSizeAnchor>
+  <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
+    <cdr:from>
+      <cdr:x>0.52215</cdr:x>
+      <cdr:y>0.79844</cdr:y>
+    </cdr:from>
+    <cdr:to>
+      <cdr:x>1</cdr:x>
+      <cdr:y>0.84787</cdr:y>
+    </cdr:to>
+    <cdr:sp macro="" textlink="">
+      <cdr:nvSpPr>
+        <cdr:cNvPr id="6" name="TextBox 5"/>
+        <cdr:cNvSpPr txBox="1"/>
+      </cdr:nvSpPr>
+      <cdr:spPr>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="4523016" y="5014149"/>
+          <a:ext cx="4139260" cy="310444"/>
+        </a:xfrm>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </cdr:spPr>
+      <cdr:txBody>
+        <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" vertOverflow="clip" wrap="none" rtlCol="0"/>
+        <a:lstStyle xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
+        <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Best Scenario - 16 Pages, page size 16, 4 cpus. First Come</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> First Serve</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+      </cdr:txBody>
+    </cdr:sp>
+  </cdr:relSizeAnchor>
+</c:userShapes>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2389,15 +2504,10 @@
   <dimension ref="A1:F55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" activeCellId="1" sqref="A2:A55 C2:C55"/>
+      <selection activeCell="A2" sqref="A2:B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">

</xml_diff>